<commit_message>
Excel code added and RFC code added
</commit_message>
<xml_diff>
--- a/Valid_ImportTemplate/Country WSP Price 2022 Spring-Summer.xlsx
+++ b/Valid_ImportTemplate/Country WSP Price 2022 Spring-Summer.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Article Number</t>
   </si>
@@ -219,6 +219,27 @@
   </si>
   <si>
     <t>14</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>82</t>
   </si>
 </sst>
 </file>
@@ -587,7 +608,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -598,7 +619,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -609,7 +630,7 @@
         <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -620,7 +641,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>